<commit_message>
CIR-1752: update service guide errors, changelog
</commit_message>
<xml_diff>
--- a/source/downloads/error-messages/Abbreviated Return Errors.xlsx
+++ b/source/downloads/error-messages/Abbreviated Return Errors.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="99">
   <si>
     <t>Error Code</t>
   </si>
@@ -73,10 +73,10 @@
     <t>Country code must be 2 letters</t>
   </si>
   <si>
-    <t>DATE_INVALID</t>
-  </si>
-  <si>
-    <t>Dates must be in the range 1900-01-01 to 2099-12-31</t>
+    <t>COUNTRY_CODE_SHOULD_NOT_BE_ENTERED</t>
+  </si>
+  <si>
+    <t>Country code should not be entered if GB, use a UTR instead</t>
   </si>
   <si>
     <t>DEEMED_EMPTY</t>
@@ -97,16 +97,22 @@
     <t>Minimum number of deemed parents is 2</t>
   </si>
   <si>
+    <t>DEEMED_PARENT_COUNTRY</t>
+  </si>
+  <si>
+    <t>Enter a country of incorporation where the deemed parent is non-UK</t>
+  </si>
+  <si>
     <t>DEEMED_PARENT_DETAILS</t>
   </si>
   <si>
     <t>Deemed parent must have either a CTUTR, a SAUTR or a country code</t>
   </si>
   <si>
-    <t>DEEMED_PARENT_UK</t>
-  </si>
-  <si>
-    <t>A UK deemed parent must have either a CTUTR or a SAUTR</t>
+    <t>DEEMED_PARENT_UTR</t>
+  </si>
+  <si>
+    <t>Enter a UTR where the deemed parent is UK</t>
   </si>
   <si>
     <t>END_DATE_18_MONTHS</t>
@@ -178,7 +184,13 @@
     <t>INVESTOR_GROUPS_SUPPLIED</t>
   </si>
   <si>
-    <t>Group ratio not elected so supply investor group not required</t>
+    <t>Group ratio blended not elected so supply investor group not required</t>
+  </si>
+  <si>
+    <t>JSON_VALIDATION_ERROR</t>
+  </si>
+  <si>
+    <t>Valid submission types are original and revised</t>
   </si>
   <si>
     <t>LEI_CHARACTER</t>
@@ -190,7 +202,7 @@
     <t>PARENT_COMPANY_NOT_SUPPLIED</t>
   </si>
   <si>
-    <t>Reporting company is not the ultimate parent, so details of ultimate parent needed</t>
+    <t>Reporting company is not the ultimate parent, so details of ultimate parent or deemed parent needed</t>
   </si>
   <si>
     <t>PARENT_COMPANY_SUPPLIED</t>
@@ -208,7 +220,7 @@
     <t>PARTNERSHIPS_EMPTY</t>
   </si>
   <si>
-    <t>Interest allowance (non-consolidated partnerships) election made, enter details of at least 1 non-consolidated partnership</t>
+    <t>Interest allowance (consolidated partnerships) election made, enter details of at least 1 consolidated partnership</t>
   </si>
   <si>
     <t>PARTNERSHIPS_NOT_SUPPLIED</t>
@@ -217,7 +229,7 @@
     <t>PARTNERSHIPS_SUPPLIED</t>
   </si>
   <si>
-    <t>Interest allowance (non-consolidated partnerships) election not made, so no details of non-consolidated partnership needed</t>
+    <t>Interest allowance (consolidated partnerships) election not made, so no details of consolidated partnership needed</t>
   </si>
   <si>
     <t>REPORTING_COMPANY_NOT_APPOINTED</t>
@@ -226,6 +238,12 @@
     <t>Reporting company required</t>
   </si>
   <si>
+    <t>RETURN_DECLARATION_FALSE</t>
+  </si>
+  <si>
+    <t>Declaration is not valid so will not be submitted. You need to confirm that the return is correct and complete to the best of your knowledge</t>
+  </si>
+  <si>
     <t>REVISION_DETAILS_CHARACTERS</t>
   </si>
   <si>
@@ -265,19 +283,13 @@
     <t>ULTIMATE_DETAILS</t>
   </si>
   <si>
-    <t>Parent company must have either a CTUTR, a SAUTR or a country code</t>
+    <t>Ultimate parent must have either a CTUTR, a SAUTR or a country code</t>
   </si>
   <si>
     <t>ULTIMATE_PARENT_COUNTRY</t>
   </si>
   <si>
     <t>Enter a country of incorporation where the ultimate parent is non-UK</t>
-  </si>
-  <si>
-    <t>ULTIMATE_PARENT_NOT_SUPPLIED</t>
-  </si>
-  <si>
-    <t>Ultimate parent company must be entered if it is not the same as the reporting company</t>
   </si>
   <si>
     <t>ULTIMATE_PARENT_UTR</t>
@@ -302,7 +314,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -317,10 +329,24 @@
     <font>
       <sz val="10.0"/>
       <color theme="1"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF0451A5"/>
+      <name val="Menlo"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,6 +359,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFE"/>
+        <bgColor rgb="FFFFFFFE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -340,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -359,7 +391,22 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -580,8 +627,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="40.43"/>
-    <col customWidth="1" min="2" max="2" width="105.71"/>
+    <col customWidth="1" min="1" max="1" width="44.86"/>
+    <col customWidth="1" min="2" max="2" width="116.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -853,27 +900,27 @@
         <v>66</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="37">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -881,7 +928,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -889,7 +936,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B39" s="4" t="s">
@@ -929,7 +976,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B44" s="4" t="s">
@@ -945,7 +992,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -953,7 +1000,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B47" s="4" t="s">
@@ -961,7 +1008,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -969,248 +1016,242 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="6"/>
-      <c r="B49" s="4"/>
+      <c r="A49" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="6"/>
-      <c r="B50" s="4"/>
+      <c r="A50" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="6"/>
-      <c r="B51" s="4"/>
+      <c r="B51" s="7"/>
     </row>
     <row r="52">
-      <c r="A52" s="6"/>
-      <c r="B52" s="4"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="7"/>
     </row>
     <row r="53">
-      <c r="A53" s="6"/>
-      <c r="B53" s="4"/>
+      <c r="B53" s="7"/>
     </row>
     <row r="54">
-      <c r="A54" s="6"/>
-      <c r="B54" s="4"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="7"/>
     </row>
     <row r="55">
-      <c r="A55" s="6"/>
-      <c r="B55" s="4"/>
+      <c r="A55" s="10"/>
+      <c r="B55" s="7"/>
     </row>
     <row r="56">
-      <c r="A56" s="6"/>
-      <c r="B56" s="4"/>
+      <c r="B56" s="7"/>
     </row>
     <row r="57">
-      <c r="A57" s="6"/>
-      <c r="B57" s="4"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="7"/>
     </row>
     <row r="58">
-      <c r="A58" s="6"/>
-      <c r="B58" s="4"/>
+      <c r="A58" s="11"/>
+      <c r="B58" s="7"/>
     </row>
     <row r="59">
-      <c r="A59" s="6"/>
-      <c r="B59" s="4"/>
+      <c r="A59" s="11"/>
+      <c r="B59" s="7"/>
     </row>
     <row r="60">
-      <c r="A60" s="5"/>
-      <c r="B60" s="4"/>
+      <c r="A60" s="11"/>
+      <c r="B60" s="7"/>
     </row>
     <row r="61">
-      <c r="A61" s="5"/>
-      <c r="B61" s="4"/>
+      <c r="A61" s="11"/>
+      <c r="B61" s="7"/>
     </row>
     <row r="62">
-      <c r="A62" s="5"/>
-      <c r="B62" s="4"/>
+      <c r="A62" s="11"/>
+      <c r="B62" s="7"/>
     </row>
     <row r="63">
-      <c r="A63" s="5"/>
-      <c r="B63" s="4"/>
+      <c r="A63" s="11"/>
+      <c r="B63" s="7"/>
     </row>
     <row r="64">
-      <c r="A64" s="5"/>
-      <c r="B64" s="4"/>
+      <c r="A64" s="11"/>
+      <c r="B64" s="7"/>
     </row>
     <row r="65">
-      <c r="A65" s="5"/>
-      <c r="B65" s="4"/>
+      <c r="A65" s="11"/>
+      <c r="B65" s="7"/>
     </row>
     <row r="66">
-      <c r="A66" s="5"/>
-      <c r="B66" s="4"/>
+      <c r="A66" s="11"/>
+      <c r="B66" s="7"/>
     </row>
     <row r="67">
-      <c r="A67" s="5"/>
-      <c r="B67" s="4"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="7"/>
     </row>
     <row r="68">
-      <c r="A68" s="5"/>
-      <c r="B68" s="4"/>
+      <c r="A68" s="10"/>
+      <c r="B68" s="7"/>
     </row>
     <row r="69">
-      <c r="A69" s="5"/>
-      <c r="B69" s="4"/>
+      <c r="A69" s="10"/>
+      <c r="B69" s="7"/>
     </row>
     <row r="70">
-      <c r="A70" s="6"/>
-      <c r="B70" s="4"/>
+      <c r="A70" s="10"/>
+      <c r="B70" s="7"/>
     </row>
     <row r="71">
-      <c r="A71" s="6"/>
-      <c r="B71" s="4"/>
+      <c r="A71" s="10"/>
+      <c r="B71" s="7"/>
     </row>
     <row r="72">
-      <c r="A72" s="6"/>
-      <c r="B72" s="4"/>
+      <c r="A72" s="10"/>
+      <c r="B72" s="7"/>
     </row>
     <row r="73">
-      <c r="A73" s="6"/>
-      <c r="B73" s="4"/>
+      <c r="A73" s="10"/>
+      <c r="B73" s="7"/>
     </row>
     <row r="74">
-      <c r="A74" s="6"/>
-      <c r="B74" s="4"/>
+      <c r="A74" s="10"/>
+      <c r="B74" s="7"/>
     </row>
     <row r="75">
-      <c r="A75" s="6"/>
-      <c r="B75" s="4"/>
+      <c r="A75" s="10"/>
+      <c r="B75" s="7"/>
     </row>
     <row r="76">
-      <c r="A76" s="6"/>
-      <c r="B76" s="4"/>
+      <c r="A76" s="10"/>
+      <c r="B76" s="7"/>
     </row>
     <row r="77">
-      <c r="A77" s="6"/>
-      <c r="B77" s="4"/>
+      <c r="A77" s="10"/>
+      <c r="B77" s="7"/>
     </row>
     <row r="78">
-      <c r="A78" s="6"/>
-      <c r="B78" s="4"/>
+      <c r="A78" s="10"/>
+      <c r="B78" s="7"/>
     </row>
     <row r="79">
-      <c r="A79" s="6"/>
-      <c r="B79" s="4"/>
+      <c r="A79" s="10"/>
+      <c r="B79" s="7"/>
     </row>
     <row r="80">
-      <c r="A80" s="6"/>
-      <c r="B80" s="4"/>
+      <c r="A80" s="10"/>
+      <c r="B80" s="7"/>
     </row>
     <row r="81">
-      <c r="A81" s="6"/>
-      <c r="B81" s="4"/>
+      <c r="A81" s="10"/>
+      <c r="B81" s="7"/>
     </row>
     <row r="82">
-      <c r="A82" s="6"/>
-      <c r="B82" s="4"/>
+      <c r="A82" s="10"/>
+      <c r="B82" s="7"/>
     </row>
     <row r="83">
-      <c r="A83" s="6"/>
-      <c r="B83" s="4"/>
+      <c r="A83" s="11"/>
+      <c r="B83" s="7"/>
     </row>
     <row r="84">
-      <c r="A84" s="6"/>
-      <c r="B84" s="4"/>
+      <c r="A84" s="11"/>
+      <c r="B84" s="7"/>
     </row>
     <row r="85">
-      <c r="A85" s="6"/>
-      <c r="B85" s="4"/>
+      <c r="A85" s="11"/>
+      <c r="B85" s="7"/>
     </row>
     <row r="86">
-      <c r="A86" s="5"/>
-      <c r="B86" s="4"/>
+      <c r="A86" s="11"/>
+      <c r="B86" s="7"/>
     </row>
     <row r="87">
-      <c r="A87" s="5"/>
-      <c r="B87" s="4"/>
+      <c r="A87" s="11"/>
+      <c r="B87" s="7"/>
     </row>
     <row r="88">
-      <c r="A88" s="5"/>
-      <c r="B88" s="4"/>
+      <c r="A88" s="11"/>
+      <c r="B88" s="7"/>
     </row>
     <row r="89">
-      <c r="A89" s="5"/>
-      <c r="B89" s="4"/>
+      <c r="A89" s="11"/>
+      <c r="B89" s="7"/>
     </row>
     <row r="90">
-      <c r="A90" s="5"/>
-      <c r="B90" s="4"/>
+      <c r="A90" s="11"/>
+      <c r="B90" s="7"/>
     </row>
     <row r="91">
-      <c r="A91" s="5"/>
-      <c r="B91" s="4"/>
+      <c r="A91" s="11"/>
+      <c r="B91" s="7"/>
     </row>
     <row r="92">
-      <c r="A92" s="5"/>
-      <c r="B92" s="4"/>
+      <c r="A92" s="11"/>
+      <c r="B92" s="7"/>
     </row>
     <row r="93">
-      <c r="A93" s="5"/>
-      <c r="B93" s="4"/>
+      <c r="A93" s="10"/>
+      <c r="B93" s="7"/>
     </row>
     <row r="94">
-      <c r="A94" s="5"/>
-      <c r="B94" s="4"/>
+      <c r="A94" s="8"/>
+      <c r="B94" s="7"/>
     </row>
     <row r="95">
-      <c r="A95" s="5"/>
-      <c r="B95" s="4"/>
+      <c r="A95" s="8"/>
+      <c r="B95" s="7"/>
     </row>
     <row r="96">
-      <c r="A96" s="6"/>
-      <c r="B96" s="4"/>
+      <c r="A96" s="8"/>
+      <c r="B96" s="7"/>
     </row>
     <row r="97">
-      <c r="A97" s="3"/>
-      <c r="B97" s="4"/>
+      <c r="A97" s="11"/>
+      <c r="B97" s="7"/>
     </row>
     <row r="98">
-      <c r="A98" s="3"/>
-      <c r="B98" s="4"/>
+      <c r="A98" s="11"/>
+      <c r="B98" s="7"/>
     </row>
     <row r="99">
-      <c r="A99" s="3"/>
-      <c r="B99" s="4"/>
+      <c r="A99" s="11"/>
+      <c r="B99" s="7"/>
     </row>
     <row r="100">
-      <c r="A100" s="5"/>
-      <c r="B100" s="4"/>
+      <c r="A100" s="11"/>
+      <c r="B100" s="7"/>
     </row>
     <row r="101">
-      <c r="A101" s="5"/>
-      <c r="B101" s="4"/>
+      <c r="A101" s="11"/>
+      <c r="B101" s="7"/>
     </row>
     <row r="102">
-      <c r="A102" s="5"/>
-      <c r="B102" s="4"/>
+      <c r="A102" s="11"/>
+      <c r="B102" s="7"/>
     </row>
     <row r="103">
-      <c r="A103" s="5"/>
-      <c r="B103" s="4"/>
+      <c r="A103" s="11"/>
+      <c r="B103" s="7"/>
     </row>
     <row r="104">
-      <c r="A104" s="5"/>
-      <c r="B104" s="4"/>
+      <c r="A104" s="11"/>
+      <c r="B104" s="7"/>
     </row>
     <row r="105">
-      <c r="A105" s="5"/>
-      <c r="B105" s="4"/>
+      <c r="A105" s="11"/>
+      <c r="B105" s="7"/>
     </row>
     <row r="106">
-      <c r="A106" s="5"/>
-      <c r="B106" s="4"/>
-    </row>
-    <row r="107">
-      <c r="A107" s="5"/>
-      <c r="B107" s="4"/>
-    </row>
-    <row r="108">
-      <c r="A108" s="5"/>
-      <c r="B108" s="4"/>
-    </row>
-    <row r="109">
-      <c r="A109" s="3"/>
-      <c r="B109" s="4"/>
+      <c r="A106" s="8"/>
+      <c r="B106" s="7"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
CIR-1755-Update formats for xlsx templates
</commit_message>
<xml_diff>
--- a/source/downloads/error-messages/Abbreviated Return Errors.xlsx
+++ b/source/downloads/error-messages/Abbreviated Return Errors.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamcooper/Documents/GitHub/irr-api-end-to-end-service-guide/source/downloads/error-messages/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F7DE54-AB5D-224B-A40E-1E7D5D098290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Abbreviated Return Errors" sheetId="1" r:id="rId4"/>
+    <sheet name="Abbreviated Return Errors" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -313,114 +322,102 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF0451A5"/>
       <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFE"/>
-        <bgColor rgb="FFFFFFFE"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -610,28 +607,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFF4CCCC"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="44.86"/>
-    <col customWidth="1" min="2" max="2" width="116.57"/>
+    <col min="1" max="1" width="44.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="116.5" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="14.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -639,621 +640,621 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="5" t="s">
+    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="5" t="s">
+    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="5" t="s">
+    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="5" t="s">
+    <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="5" t="s">
+    <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="5" t="s">
+    <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="6"/>
       <c r="B51" s="7"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="8"/>
       <c r="B52" s="7"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="7"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="9"/>
       <c r="B54" s="7"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="10"/>
       <c r="B55" s="7"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="B56" s="7"/>
     </row>
-    <row r="57">
-      <c r="A57" s="11"/>
+    <row r="57" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A57" s="8"/>
       <c r="B57" s="7"/>
     </row>
-    <row r="58">
-      <c r="A58" s="11"/>
+    <row r="58" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A58" s="8"/>
       <c r="B58" s="7"/>
     </row>
-    <row r="59">
-      <c r="A59" s="11"/>
+    <row r="59" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A59" s="8"/>
       <c r="B59" s="7"/>
     </row>
-    <row r="60">
-      <c r="A60" s="11"/>
+    <row r="60" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A60" s="8"/>
       <c r="B60" s="7"/>
     </row>
-    <row r="61">
-      <c r="A61" s="11"/>
+    <row r="61" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A61" s="8"/>
       <c r="B61" s="7"/>
     </row>
-    <row r="62">
-      <c r="A62" s="11"/>
+    <row r="62" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A62" s="8"/>
       <c r="B62" s="7"/>
     </row>
-    <row r="63">
-      <c r="A63" s="11"/>
+    <row r="63" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A63" s="8"/>
       <c r="B63" s="7"/>
     </row>
-    <row r="64">
-      <c r="A64" s="11"/>
+    <row r="64" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A64" s="8"/>
       <c r="B64" s="7"/>
     </row>
-    <row r="65">
-      <c r="A65" s="11"/>
+    <row r="65" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A65" s="8"/>
       <c r="B65" s="7"/>
     </row>
-    <row r="66">
-      <c r="A66" s="11"/>
+    <row r="66" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A66" s="8"/>
       <c r="B66" s="7"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="10"/>
       <c r="B67" s="7"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="10"/>
       <c r="B68" s="7"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="10"/>
       <c r="B69" s="7"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="10"/>
       <c r="B70" s="7"/>
     </row>
-    <row r="71">
+    <row r="71" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="10"/>
       <c r="B71" s="7"/>
     </row>
-    <row r="72">
+    <row r="72" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="10"/>
       <c r="B72" s="7"/>
     </row>
-    <row r="73">
+    <row r="73" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="10"/>
       <c r="B73" s="7"/>
     </row>
-    <row r="74">
+    <row r="74" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="10"/>
       <c r="B74" s="7"/>
     </row>
-    <row r="75">
+    <row r="75" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="10"/>
       <c r="B75" s="7"/>
     </row>
-    <row r="76">
+    <row r="76" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="10"/>
       <c r="B76" s="7"/>
     </row>
-    <row r="77">
+    <row r="77" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="10"/>
       <c r="B77" s="7"/>
     </row>
-    <row r="78">
+    <row r="78" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="10"/>
       <c r="B78" s="7"/>
     </row>
-    <row r="79">
+    <row r="79" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="10"/>
       <c r="B79" s="7"/>
     </row>
-    <row r="80">
+    <row r="80" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="10"/>
       <c r="B80" s="7"/>
     </row>
-    <row r="81">
+    <row r="81" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="10"/>
       <c r="B81" s="7"/>
     </row>
-    <row r="82">
+    <row r="82" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="10"/>
       <c r="B82" s="7"/>
     </row>
-    <row r="83">
-      <c r="A83" s="11"/>
+    <row r="83" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A83" s="8"/>
       <c r="B83" s="7"/>
     </row>
-    <row r="84">
-      <c r="A84" s="11"/>
+    <row r="84" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A84" s="8"/>
       <c r="B84" s="7"/>
     </row>
-    <row r="85">
-      <c r="A85" s="11"/>
+    <row r="85" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A85" s="8"/>
       <c r="B85" s="7"/>
     </row>
-    <row r="86">
-      <c r="A86" s="11"/>
+    <row r="86" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A86" s="8"/>
       <c r="B86" s="7"/>
     </row>
-    <row r="87">
-      <c r="A87" s="11"/>
+    <row r="87" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A87" s="8"/>
       <c r="B87" s="7"/>
     </row>
-    <row r="88">
-      <c r="A88" s="11"/>
+    <row r="88" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A88" s="8"/>
       <c r="B88" s="7"/>
     </row>
-    <row r="89">
-      <c r="A89" s="11"/>
+    <row r="89" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A89" s="8"/>
       <c r="B89" s="7"/>
     </row>
-    <row r="90">
-      <c r="A90" s="11"/>
+    <row r="90" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A90" s="8"/>
       <c r="B90" s="7"/>
     </row>
-    <row r="91">
-      <c r="A91" s="11"/>
+    <row r="91" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A91" s="8"/>
       <c r="B91" s="7"/>
     </row>
-    <row r="92">
-      <c r="A92" s="11"/>
+    <row r="92" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A92" s="8"/>
       <c r="B92" s="7"/>
     </row>
-    <row r="93">
+    <row r="93" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="10"/>
       <c r="B93" s="7"/>
     </row>
-    <row r="94">
+    <row r="94" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="8"/>
       <c r="B94" s="7"/>
     </row>
-    <row r="95">
+    <row r="95" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="8"/>
       <c r="B95" s="7"/>
     </row>
-    <row r="96">
+    <row r="96" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="8"/>
       <c r="B96" s="7"/>
     </row>
-    <row r="97">
-      <c r="A97" s="11"/>
+    <row r="97" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A97" s="8"/>
       <c r="B97" s="7"/>
     </row>
-    <row r="98">
-      <c r="A98" s="11"/>
+    <row r="98" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A98" s="8"/>
       <c r="B98" s="7"/>
     </row>
-    <row r="99">
-      <c r="A99" s="11"/>
+    <row r="99" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A99" s="8"/>
       <c r="B99" s="7"/>
     </row>
-    <row r="100">
-      <c r="A100" s="11"/>
+    <row r="100" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A100" s="8"/>
       <c r="B100" s="7"/>
     </row>
-    <row r="101">
-      <c r="A101" s="11"/>
+    <row r="101" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A101" s="8"/>
       <c r="B101" s="7"/>
     </row>
-    <row r="102">
-      <c r="A102" s="11"/>
+    <row r="102" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A102" s="8"/>
       <c r="B102" s="7"/>
     </row>
-    <row r="103">
-      <c r="A103" s="11"/>
+    <row r="103" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A103" s="8"/>
       <c r="B103" s="7"/>
     </row>
-    <row r="104">
-      <c r="A104" s="11"/>
+    <row r="104" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A104" s="8"/>
       <c r="B104" s="7"/>
     </row>
-    <row r="105">
-      <c r="A105" s="11"/>
+    <row r="105" spans="1:2" ht="13" x14ac:dyDescent="0.15">
+      <c r="A105" s="8"/>
       <c r="B105" s="7"/>
     </row>
-    <row r="106">
+    <row r="106" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="8"/>
       <c r="B106" s="7"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CIR-1761-Updated xlsx sheets for full and abb return errors
</commit_message>
<xml_diff>
--- a/source/downloads/error-messages/Abbreviated Return Errors.xlsx
+++ b/source/downloads/error-messages/Abbreviated Return Errors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamcooper/Documents/GitHub/irr-api-end-to-end-service-guide/source/downloads/error-messages/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F7DE54-AB5D-224B-A40E-1E7D5D098290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BDE1EF-B190-2A44-A5A1-3CEF7A57E8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -145,9 +145,6 @@
     <t>GROUP_RATIO_BLENDED_NOT_SUPPLIED</t>
   </si>
   <si>
-    <t>If group ratio is elected, a value for group ratio (blended) election must be provided</t>
-  </si>
-  <si>
     <t>GROUP_RATIO_BLENDED_SUPPLIED</t>
   </si>
   <si>
@@ -317,6 +314,9 @@
   </si>
   <si>
     <t>UTR must be 10 numeric characters</t>
+  </si>
+  <si>
+    <t>If group ratio % is elected, a value for group ratio (blended) election must be true or false</t>
   </si>
 </sst>
 </file>
@@ -622,7 +622,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -797,239 +797,239 @@
         <v>40</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>